<commit_message>
pushing draft from Wed of Proj 2
</commit_message>
<xml_diff>
--- a/Project2/data/StudentEvaluation- TO PREDICT.xlsx
+++ b/Project2/data/StudentEvaluation- TO PREDICT.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\!SB\!CUNY\!! Fall 2017 Term\624 Predictive Analytics\Project #2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1c4ee0090c546ac9/Master Of Data Science - CUNY/Summer 2021/Predictive_Analytics/Predictive-Analytics/Project2/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_EB861AA7F646CE41779813C0E3825DABCBC800AE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AD543012-2EE3-47E7-8F2D-CC281D2EFD9C}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="105" windowWidth="19155" windowHeight="12300"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Subset (2)" sheetId="1" r:id="rId1"/>
@@ -135,7 +136,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -163,7 +164,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
@@ -266,6 +267,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -359,6 +361,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -394,6 +413,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -569,11 +605,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AG268"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="Z2" sqref="Z2:Z290"/>
+    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="U18" sqref="U18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -784,6 +820,9 @@
       <c r="Y2" s="24">
         <v>-3.8</v>
       </c>
+      <c r="Z2" s="34">
+        <v>-0.55650776624679599</v>
+      </c>
       <c r="AA2" s="26">
         <v>2.1999999999999999E-2</v>
       </c>
@@ -882,6 +921,9 @@
       <c r="Y3" s="24">
         <v>-4.4000000000000004</v>
       </c>
+      <c r="Z3" s="34">
+        <v>0.101060643792152</v>
+      </c>
       <c r="AA3" s="26">
         <v>0.03</v>
       </c>
@@ -980,6 +1022,9 @@
       <c r="Y4" s="24">
         <v>-4.2</v>
       </c>
+      <c r="Z4" s="34">
+        <v>0.49030539393424999</v>
+      </c>
       <c r="AA4" s="26">
         <v>4.5999999999999999E-2</v>
       </c>
@@ -1072,6 +1117,9 @@
       <c r="Y5" s="24">
         <v>-4</v>
       </c>
+      <c r="Z5" s="34">
+        <v>0.60111629962921098</v>
+      </c>
       <c r="AB5" s="27">
         <v>120</v>
       </c>
@@ -1167,6 +1215,9 @@
       <c r="Y6" s="24">
         <v>-4</v>
       </c>
+      <c r="Z6" s="34">
+        <v>1.1963568627834299E-2</v>
+      </c>
       <c r="AA6" s="26">
         <v>8.2000000000000003E-2</v>
       </c>
@@ -1262,6 +1313,9 @@
       <c r="Y7" s="24">
         <v>-3.8</v>
       </c>
+      <c r="Z7" s="34">
+        <v>0.67511576414108299</v>
+      </c>
       <c r="AA7" s="26">
         <v>6.4000000000000001E-2</v>
       </c>
@@ -1360,6 +1414,9 @@
       <c r="Y8" s="24">
         <v>-4.2</v>
       </c>
+      <c r="Z8" s="34">
+        <v>0.106666684150696</v>
+      </c>
       <c r="AA8" s="26">
         <v>4.2000000000000003E-2</v>
       </c>
@@ -1449,6 +1506,9 @@
       <c r="Y9" s="24">
         <v>-4.4000000000000004</v>
       </c>
+      <c r="Z9" s="34">
+        <v>0.21584773063659701</v>
+      </c>
       <c r="AA9" s="26">
         <v>9.6000000000000002E-2</v>
       </c>
@@ -1547,6 +1607,9 @@
       <c r="Y10" s="24">
         <v>-4.4000000000000004</v>
       </c>
+      <c r="Z10" s="34">
+        <v>-4.2998582124710097E-2</v>
+      </c>
       <c r="AA10" s="26">
         <v>4.5999999999999999E-2</v>
       </c>
@@ -1642,6 +1705,9 @@
       <c r="Y11" s="24">
         <v>-4.2</v>
       </c>
+      <c r="Z11" s="34">
+        <v>7.43265971541405E-2</v>
+      </c>
       <c r="AA11" s="26">
         <v>9.6000000000000002E-2</v>
       </c>
@@ -1734,6 +1800,9 @@
       <c r="Y12" s="24">
         <v>-4.2</v>
       </c>
+      <c r="Z12" s="34">
+        <v>0.52231878042221103</v>
+      </c>
       <c r="AA12" s="26">
         <v>6.6000000000000003E-2</v>
       </c>
@@ -1832,6 +1901,9 @@
       <c r="Y13" s="24">
         <v>-4.2</v>
       </c>
+      <c r="Z13" s="34">
+        <v>0.51924812793731701</v>
+      </c>
       <c r="AA13" s="26">
         <v>4.8000000000000001E-2</v>
       </c>
@@ -1930,6 +2002,9 @@
       <c r="Y14" s="24">
         <v>-4.8</v>
       </c>
+      <c r="Z14" s="34">
+        <v>-0.14168371260166199</v>
+      </c>
       <c r="AA14" s="26">
         <v>6.6000000000000003E-2</v>
       </c>
@@ -2028,6 +2103,9 @@
       <c r="Y15" s="24">
         <v>-4.8</v>
       </c>
+      <c r="Z15" s="34">
+        <v>7.3170207440853105E-2</v>
+      </c>
       <c r="AA15" s="26">
         <v>0.05</v>
       </c>
@@ -2126,6 +2204,9 @@
       <c r="Y16" s="24">
         <v>-4.2</v>
       </c>
+      <c r="Z16" s="34">
+        <v>-1.46697354316711</v>
+      </c>
       <c r="AA16" s="26">
         <v>4.5999999999999999E-2</v>
       </c>
@@ -2215,6 +2296,9 @@
       <c r="Y17" s="24">
         <v>-4.8</v>
       </c>
+      <c r="Z17" s="34">
+        <v>-0.50808966159820601</v>
+      </c>
       <c r="AA17" s="26">
         <v>0.16</v>
       </c>
@@ -2313,6 +2397,9 @@
       <c r="Y18" s="24">
         <v>-4</v>
       </c>
+      <c r="Z18" s="34">
+        <v>6.8106971681117998E-2</v>
+      </c>
       <c r="AA18" s="26">
         <v>0.10199999999999999</v>
       </c>
@@ -2411,6 +2498,9 @@
       <c r="Y19" s="24">
         <v>-4.4000000000000004</v>
       </c>
+      <c r="Z19" s="34">
+        <v>-0.442760169506073</v>
+      </c>
       <c r="AA19" s="26">
         <v>0.06</v>
       </c>
@@ -2509,6 +2599,9 @@
       <c r="Y20" s="24">
         <v>-4.2</v>
       </c>
+      <c r="Z20" s="34">
+        <v>-0.52099192142486594</v>
+      </c>
       <c r="AA20" s="26">
         <v>0.154</v>
       </c>
@@ -2607,6 +2700,9 @@
       <c r="Y21" s="24">
         <v>-4.4000000000000004</v>
       </c>
+      <c r="Z21" s="34">
+        <v>0.10242690145969401</v>
+      </c>
       <c r="AA21" s="26">
         <v>2.1999999999999999E-2</v>
       </c>
@@ -2705,6 +2801,9 @@
       <c r="Y22" s="24">
         <v>-4.4000000000000004</v>
       </c>
+      <c r="Z22" s="34">
+        <v>-0.216088116168976</v>
+      </c>
       <c r="AA22" s="26">
         <v>2.1999999999999999E-2</v>
       </c>
@@ -2800,6 +2899,9 @@
       <c r="Y23" s="24">
         <v>-4.4000000000000004</v>
       </c>
+      <c r="Z23" s="34">
+        <v>0.162890404462814</v>
+      </c>
       <c r="AA23" s="26">
         <v>5.3999999999999999E-2</v>
       </c>
@@ -2892,6 +2994,9 @@
       <c r="Y24" s="24">
         <v>-4.4000000000000004</v>
       </c>
+      <c r="Z24" s="34">
+        <v>-0.57927429676055897</v>
+      </c>
       <c r="AA24" s="26">
         <v>2.1999999999999999E-2</v>
       </c>
@@ -2990,6 +3095,9 @@
       <c r="Y25" s="24">
         <v>-4</v>
       </c>
+      <c r="Z25" s="34">
+        <v>-0.466716408729553</v>
+      </c>
       <c r="AA25" s="26">
         <v>2.1999999999999999E-2</v>
       </c>
@@ -3088,6 +3196,9 @@
       <c r="Y26" s="24">
         <v>-4.5999999999999996</v>
       </c>
+      <c r="Z26" s="34">
+        <v>-0.219779253005981</v>
+      </c>
       <c r="AA26" s="26">
         <v>2.4E-2</v>
       </c>
@@ -3186,6 +3297,9 @@
       <c r="Y27" s="24">
         <v>-4.4000000000000004</v>
       </c>
+      <c r="Z27" s="34">
+        <v>-1.2659695148468</v>
+      </c>
       <c r="AA27" s="26">
         <v>2.1999999999999999E-2</v>
       </c>
@@ -3284,6 +3398,9 @@
       <c r="Y28" s="24">
         <v>-4.2</v>
       </c>
+      <c r="Z28" s="34">
+        <v>-1.4667437076568599</v>
+      </c>
       <c r="AA28" s="26">
         <v>2.1999999999999999E-2</v>
       </c>
@@ -3382,6 +3499,9 @@
       <c r="Y29" s="24">
         <v>-3.8</v>
       </c>
+      <c r="Z29" s="34">
+        <v>-0.24552266299724601</v>
+      </c>
       <c r="AA29" s="26">
         <v>0.17399999999999999</v>
       </c>
@@ -3477,6 +3597,9 @@
       <c r="Y30" s="24">
         <v>-3.8</v>
       </c>
+      <c r="Z30" s="34">
+        <v>-0.186196699738503</v>
+      </c>
       <c r="AA30" s="26">
         <v>2.1999999999999999E-2</v>
       </c>
@@ -3575,6 +3698,9 @@
       <c r="Y31" s="24">
         <v>-4</v>
       </c>
+      <c r="Z31" s="34">
+        <v>-0.52603912353515603</v>
+      </c>
       <c r="AA31" s="26">
         <v>2.4E-2</v>
       </c>
@@ -3673,6 +3799,9 @@
       <c r="Y32" s="24">
         <v>-4</v>
       </c>
+      <c r="Z32" s="34">
+        <v>-0.649968862533569</v>
+      </c>
       <c r="AA32" s="26">
         <v>6.6000000000000003E-2</v>
       </c>
@@ -3768,6 +3897,9 @@
       <c r="Y33" s="24">
         <v>-4.2</v>
       </c>
+      <c r="Z33" s="34">
+        <v>-0.218598857522011</v>
+      </c>
       <c r="AA33" s="26">
         <v>2.4E-2</v>
       </c>
@@ -3863,6 +3995,9 @@
       <c r="Y34" s="24">
         <v>-4.2</v>
       </c>
+      <c r="Z34" s="34">
+        <v>0.12567086517810799</v>
+      </c>
       <c r="AA34" s="26">
         <v>2.1999999999999999E-2</v>
       </c>
@@ -3958,6 +4093,9 @@
       <c r="Y35" s="24">
         <v>-4.2</v>
       </c>
+      <c r="Z35" s="34">
+        <v>-0.45948278903961198</v>
+      </c>
       <c r="AA35" s="26">
         <v>2.1999999999999999E-2</v>
       </c>
@@ -4053,6 +4191,9 @@
       <c r="Y36" s="24">
         <v>-4</v>
       </c>
+      <c r="Z36" s="34">
+        <v>-0.11021700501442</v>
+      </c>
       <c r="AA36" s="26">
         <v>3.5999999999999997E-2</v>
       </c>
@@ -4151,6 +4292,9 @@
       <c r="Y37" s="24">
         <v>-4</v>
       </c>
+      <c r="Z37" s="34">
+        <v>-0.44808921217918402</v>
+      </c>
       <c r="AA37" s="26">
         <v>2.1999999999999999E-2</v>
       </c>
@@ -4249,6 +4393,9 @@
       <c r="Y38" s="24">
         <v>-3.6</v>
       </c>
+      <c r="Z38" s="34">
+        <v>-0.385998725891113</v>
+      </c>
       <c r="AA38" s="26">
         <v>2.1999999999999999E-2</v>
       </c>
@@ -4347,6 +4494,9 @@
       <c r="Y39" s="24">
         <v>-3.6</v>
       </c>
+      <c r="Z39" s="34">
+        <v>-0.53208482265472401</v>
+      </c>
       <c r="AA39" s="26">
         <v>2.1999999999999999E-2</v>
       </c>
@@ -4445,6 +4595,9 @@
       <c r="Y40" s="24">
         <v>-4.4000000000000004</v>
       </c>
+      <c r="Z40" s="34">
+        <v>-0.43826180696487399</v>
+      </c>
       <c r="AA40" s="26">
         <v>5.1999999999999998E-2</v>
       </c>
@@ -4540,6 +4693,9 @@
       <c r="Y41" s="24">
         <v>-4.4000000000000004</v>
       </c>
+      <c r="Z41" s="34">
+        <v>-1.1083890683949001E-2</v>
+      </c>
       <c r="AA41" s="26">
         <v>0.05</v>
       </c>
@@ -4638,6 +4794,9 @@
       <c r="Y42" s="24">
         <v>-4.4000000000000004</v>
       </c>
+      <c r="Z42" s="34">
+        <v>3.82725358940661E-3</v>
+      </c>
       <c r="AA42" s="26">
         <v>4.2000000000000003E-2</v>
       </c>
@@ -4733,6 +4892,9 @@
       <c r="Y43" s="24">
         <v>-4.5999999999999996</v>
       </c>
+      <c r="Z43" s="34">
+        <v>-0.918598651885986</v>
+      </c>
       <c r="AA43" s="26">
         <v>2.4E-2</v>
       </c>
@@ -4831,6 +4993,9 @@
       <c r="Y44" s="24">
         <v>-5</v>
       </c>
+      <c r="Z44" s="34">
+        <v>-1.1634151935577399</v>
+      </c>
       <c r="AA44" s="26">
         <v>2.1999999999999999E-2</v>
       </c>
@@ -4929,6 +5094,9 @@
       <c r="Y45" s="24">
         <v>-5</v>
       </c>
+      <c r="Z45" s="34">
+        <v>-0.91614741086959794</v>
+      </c>
       <c r="AA45" s="26">
         <v>2.1999999999999999E-2</v>
       </c>
@@ -5027,6 +5195,9 @@
       <c r="Y46" s="24">
         <v>-5.4</v>
       </c>
+      <c r="Z46" s="34">
+        <v>-0.14046427607536299</v>
+      </c>
       <c r="AA46" s="26">
         <v>2.4E-2</v>
       </c>
@@ -5125,6 +5296,9 @@
       <c r="Y47" s="24">
         <v>-5</v>
       </c>
+      <c r="Z47" s="34">
+        <v>0.958285331726074</v>
+      </c>
       <c r="AA47" s="26">
         <v>3.5999999999999997E-2</v>
       </c>
@@ -5223,6 +5397,9 @@
       <c r="Y48" s="24">
         <v>-5.2</v>
       </c>
+      <c r="Z48" s="34">
+        <v>1.1081281900405899</v>
+      </c>
       <c r="AA48" s="26">
         <v>3.5999999999999997E-2</v>
       </c>
@@ -5321,6 +5498,9 @@
       <c r="Y49" s="24">
         <v>-4.8</v>
       </c>
+      <c r="Z49" s="34">
+        <v>-0.276242464780807</v>
+      </c>
       <c r="AA49" s="26">
         <v>2.4E-2</v>
       </c>
@@ -5419,6 +5599,9 @@
       <c r="Y50" s="24">
         <v>-5.2</v>
       </c>
+      <c r="Z50" s="34">
+        <v>1.05038690567017</v>
+      </c>
       <c r="AA50" s="26">
         <v>2.4E-2</v>
       </c>
@@ -5517,6 +5700,9 @@
       <c r="Y51" s="24">
         <v>-4.8</v>
       </c>
+      <c r="Z51" s="34">
+        <v>0.523132264614105</v>
+      </c>
       <c r="AA51" s="26">
         <v>2.4E-2</v>
       </c>
@@ -5609,6 +5795,9 @@
       <c r="Y52" s="24">
         <v>-5.2</v>
       </c>
+      <c r="Z52" s="34">
+        <v>-0.25540363788604697</v>
+      </c>
       <c r="AA52" s="26">
         <v>7.0000000000000007E-2</v>
       </c>
@@ -5707,6 +5896,9 @@
       <c r="Y53" s="24">
         <v>-4.8</v>
       </c>
+      <c r="Z53" s="34">
+        <v>-7.2629041969776195E-2</v>
+      </c>
       <c r="AA53" s="26">
         <v>2.1999999999999999E-2</v>
       </c>
@@ -5802,6 +5994,9 @@
       <c r="Y54" s="24">
         <v>-5.2</v>
       </c>
+      <c r="Z54" s="34">
+        <v>0.69158190488815297</v>
+      </c>
       <c r="AA54" s="26">
         <v>0.122</v>
       </c>
@@ -5897,6 +6092,9 @@
       <c r="Y55" s="24">
         <v>-5</v>
       </c>
+      <c r="Z55" s="34">
+        <v>1.3487890958786</v>
+      </c>
       <c r="AA55" s="26">
         <v>2.4E-2</v>
       </c>
@@ -5995,6 +6193,9 @@
       <c r="Y56" s="24">
         <v>-5</v>
       </c>
+      <c r="Z56" s="34">
+        <v>1.47055411338806</v>
+      </c>
       <c r="AA56" s="26">
         <v>2.4E-2</v>
       </c>
@@ -6093,6 +6294,9 @@
       <c r="Y57" s="24">
         <v>-5</v>
       </c>
+      <c r="Z57" s="34">
+        <v>1.07375156879425</v>
+      </c>
       <c r="AA57" s="26">
         <v>4.2000000000000003E-2</v>
       </c>
@@ -6191,6 +6395,9 @@
       <c r="Y58" s="24">
         <v>-5.4</v>
       </c>
+      <c r="Z58" s="34">
+        <v>-0.89910638332366899</v>
+      </c>
       <c r="AA58" s="26">
         <v>0.12</v>
       </c>
@@ -6289,6 +6496,9 @@
       <c r="Y59" s="24">
         <v>-5</v>
       </c>
+      <c r="Z59" s="34">
+        <v>-0.581981420516968</v>
+      </c>
       <c r="AA59" s="26">
         <v>6.8000000000000005E-2</v>
       </c>
@@ -6387,6 +6597,9 @@
       <c r="Y60" s="24">
         <v>-5</v>
       </c>
+      <c r="Z60" s="34">
+        <v>0.92871749401092496</v>
+      </c>
       <c r="AA60" s="26">
         <v>6.6000000000000003E-2</v>
       </c>
@@ -6485,6 +6698,9 @@
       <c r="Y61" s="24">
         <v>-4.5999999999999996</v>
       </c>
+      <c r="Z61" s="34">
+        <v>1.2602424621582</v>
+      </c>
       <c r="AA61" s="26">
         <v>4.2000000000000003E-2</v>
       </c>
@@ -6583,6 +6799,9 @@
       <c r="Y62" s="24">
         <v>-4.4000000000000004</v>
       </c>
+      <c r="Z62" s="34">
+        <v>0.84630739688873302</v>
+      </c>
       <c r="AA62" s="26">
         <v>5.8000000000000003E-2</v>
       </c>
@@ -6681,6 +6900,9 @@
       <c r="Y63" s="24">
         <v>-4.8</v>
       </c>
+      <c r="Z63" s="34">
+        <v>0.65892010927200295</v>
+      </c>
       <c r="AA63" s="26">
         <v>5.8000000000000003E-2</v>
       </c>
@@ -6779,6 +7001,9 @@
       <c r="Y64" s="24">
         <v>-4.4000000000000004</v>
       </c>
+      <c r="Z64" s="34">
+        <v>1.11713087558746</v>
+      </c>
       <c r="AA64" s="26">
         <v>9.1999999999999998E-2</v>
       </c>
@@ -6877,6 +7102,9 @@
       <c r="Y65" s="24">
         <v>-4.4000000000000004</v>
       </c>
+      <c r="Z65" s="34">
+        <v>0.27316477894782998</v>
+      </c>
       <c r="AA65" s="26">
         <v>0.14599999999999999</v>
       </c>
@@ -6975,6 +7203,9 @@
       <c r="Y66" s="24">
         <v>-4.2</v>
       </c>
+      <c r="Z66" s="34">
+        <v>0.89005416631698597</v>
+      </c>
       <c r="AA66" s="26">
         <v>0.108</v>
       </c>
@@ -7073,6 +7304,9 @@
       <c r="Y67" s="24">
         <v>-4.8</v>
       </c>
+      <c r="Z67" s="34">
+        <v>1.1672108173370399</v>
+      </c>
       <c r="AA67" s="26">
         <v>0.05</v>
       </c>
@@ -7171,6 +7405,9 @@
       <c r="Y68" s="24">
         <v>-5.4</v>
       </c>
+      <c r="Z68" s="34">
+        <v>-1.28355357446708E-4</v>
+      </c>
       <c r="AA68" s="26">
         <v>0.158</v>
       </c>
@@ -7269,6 +7506,9 @@
       <c r="Y69" s="24">
         <v>-5.4</v>
       </c>
+      <c r="Z69" s="34">
+        <v>-0.20283347368240401</v>
+      </c>
       <c r="AA69" s="26">
         <v>0.13800000000000001</v>
       </c>
@@ -7367,6 +7607,9 @@
       <c r="Y70" s="24">
         <v>-5.6</v>
       </c>
+      <c r="Z70" s="34">
+        <v>-3.8983177393674899E-2</v>
+      </c>
       <c r="AA70" s="26">
         <v>0.13200000000000001</v>
       </c>
@@ -7465,6 +7708,9 @@
       <c r="Y71" s="24">
         <v>-5.4</v>
       </c>
+      <c r="Z71" s="34">
+        <v>-1.9833680242299999E-2</v>
+      </c>
       <c r="AA71" s="26">
         <v>0.17199999999999999</v>
       </c>
@@ -7563,6 +7809,9 @@
       <c r="Y72" s="24">
         <v>-5.2</v>
       </c>
+      <c r="Z72" s="34">
+        <v>-0.92650467157363903</v>
+      </c>
       <c r="AA72" s="26">
         <v>0.22</v>
       </c>
@@ -7661,6 +7910,9 @@
       <c r="Y73" s="24">
         <v>-5.4</v>
       </c>
+      <c r="Z73" s="34">
+        <v>-1.53037405014038</v>
+      </c>
       <c r="AA73" s="26">
         <v>0.126</v>
       </c>
@@ -7759,6 +8011,9 @@
       <c r="Y74" s="24">
         <v>-5.8</v>
       </c>
+      <c r="Z74" s="34">
+        <v>-9.5955476164817796E-2</v>
+      </c>
       <c r="AA74" s="26">
         <v>8.5999999999999993E-2</v>
       </c>
@@ -7857,6 +8112,9 @@
       <c r="Y75" s="24">
         <v>-5.8</v>
       </c>
+      <c r="Z75" s="34">
+        <v>-0.82861459255218495</v>
+      </c>
       <c r="AA75" s="26">
         <v>0.11600000000000001</v>
       </c>
@@ -7955,6 +8213,9 @@
       <c r="Y76" s="24">
         <v>-5.6</v>
       </c>
+      <c r="Z76" s="34">
+        <v>-0.15096455812454199</v>
+      </c>
       <c r="AA76" s="26">
         <v>6.8000000000000005E-2</v>
       </c>
@@ -8053,6 +8314,9 @@
       <c r="Y77" s="24">
         <v>-5.6</v>
       </c>
+      <c r="Z77" s="34">
+        <v>-0.54225599765777599</v>
+      </c>
       <c r="AA77" s="26">
         <v>0.06</v>
       </c>
@@ -8151,6 +8415,9 @@
       <c r="Y78" s="24">
         <v>-5.8</v>
       </c>
+      <c r="Z78" s="34">
+        <v>0.277163326740265</v>
+      </c>
       <c r="AA78" s="26">
         <v>4.3999999999999997E-2</v>
       </c>
@@ -8246,6 +8513,9 @@
       <c r="Y79" s="24">
         <v>-5</v>
       </c>
+      <c r="Z79" s="34">
+        <v>0.25786042213439903</v>
+      </c>
       <c r="AA79" s="26">
         <v>7.5999999999999998E-2</v>
       </c>
@@ -8344,6 +8614,9 @@
       <c r="Y80" s="24">
         <v>-5.4</v>
       </c>
+      <c r="Z80" s="34">
+        <v>1.0257149934768699</v>
+      </c>
       <c r="AA80" s="26">
         <v>5.8000000000000003E-2</v>
       </c>
@@ -8442,6 +8715,9 @@
       <c r="Y81" s="24">
         <v>-5.4</v>
       </c>
+      <c r="Z81" s="34">
+        <v>-0.41667845845222501</v>
+      </c>
       <c r="AA81" s="26">
         <v>5.1999999999999998E-2</v>
       </c>
@@ -8540,6 +8816,9 @@
       <c r="Y82" s="24">
         <v>-5.4</v>
       </c>
+      <c r="Z82" s="34">
+        <v>0.30153110623359702</v>
+      </c>
       <c r="AA82" s="26">
         <v>7.0000000000000007E-2</v>
       </c>
@@ -8638,6 +8917,9 @@
       <c r="Y83" s="24">
         <v>-4.4000000000000004</v>
       </c>
+      <c r="Z83" s="34">
+        <v>1.0245211124420199</v>
+      </c>
       <c r="AA83" s="26">
         <v>0.16800000000000001</v>
       </c>
@@ -8736,6 +9018,9 @@
       <c r="Y84" s="24">
         <v>-4.4000000000000004</v>
       </c>
+      <c r="Z84" s="34">
+        <v>1.5948728322982799</v>
+      </c>
       <c r="AA84" s="26">
         <v>0.17</v>
       </c>
@@ -8834,6 +9119,9 @@
       <c r="Y85" s="24">
         <v>-4.4000000000000004</v>
       </c>
+      <c r="Z85" s="34">
+        <v>1.0377233028411901</v>
+      </c>
       <c r="AA85" s="26">
         <v>0.09</v>
       </c>
@@ -8923,6 +9211,9 @@
       <c r="Y86" s="24">
         <v>-4.2</v>
       </c>
+      <c r="Z86" s="34">
+        <v>1.1080392599105799</v>
+      </c>
       <c r="AB86" s="27">
         <v>120</v>
       </c>
@@ -9015,6 +9306,9 @@
       <c r="Y87" s="24">
         <v>-5</v>
       </c>
+      <c r="Z87" s="34">
+        <v>0.95120108127594005</v>
+      </c>
       <c r="AA87" s="26">
         <v>6.8000000000000005E-2</v>
       </c>
@@ -9113,6 +9407,9 @@
       <c r="Y88" s="24">
         <v>-5</v>
       </c>
+      <c r="Z88" s="34">
+        <v>0.92444282770156905</v>
+      </c>
       <c r="AA88" s="26">
         <v>4.5999999999999999E-2</v>
       </c>
@@ -9211,6 +9508,9 @@
       <c r="Y89" s="24">
         <v>-5.8</v>
       </c>
+      <c r="Z89" s="34">
+        <v>-0.60640394687652599</v>
+      </c>
       <c r="AA89" s="26">
         <v>6.6000000000000003E-2</v>
       </c>
@@ -9309,6 +9609,9 @@
       <c r="Y90" s="24">
         <v>-5.8</v>
       </c>
+      <c r="Z90" s="34">
+        <v>-0.62371188402175903</v>
+      </c>
       <c r="AA90" s="26">
         <v>0.19400000000000001</v>
       </c>
@@ -9407,6 +9710,9 @@
       <c r="Y91" s="24">
         <v>-5.4</v>
       </c>
+      <c r="Z91" s="34">
+        <v>0.94632053375244096</v>
+      </c>
       <c r="AA91" s="26">
         <v>8.2000000000000003E-2</v>
       </c>
@@ -9502,6 +9808,9 @@
       <c r="Y92" s="24">
         <v>-5.2</v>
       </c>
+      <c r="Z92" s="34">
+        <v>0.258763998746872</v>
+      </c>
       <c r="AA92" s="26">
         <v>8.4000000000000005E-2</v>
       </c>
@@ -9573,6 +9882,9 @@
       <c r="X93" s="23">
         <v>3.48</v>
       </c>
+      <c r="Z93" s="34">
+        <v>-0.95387440919876099</v>
+      </c>
       <c r="AC93" s="28">
         <v>46</v>
       </c>
@@ -9656,6 +9968,9 @@
       <c r="Y94" s="24">
         <v>-5.8</v>
       </c>
+      <c r="Z94" s="34">
+        <v>-0.69708615541458097</v>
+      </c>
       <c r="AA94" s="26">
         <v>0.35399999999999998</v>
       </c>
@@ -9751,6 +10066,9 @@
       <c r="Y95" s="24">
         <v>-5.8</v>
       </c>
+      <c r="Z95" s="34">
+        <v>-0.64580619335174605</v>
+      </c>
       <c r="AA95" s="26">
         <v>0.39800000000000002</v>
       </c>
@@ -9846,6 +10164,9 @@
       <c r="Y96" s="24">
         <v>-5.4</v>
       </c>
+      <c r="Z96" s="34">
+        <v>0.32253432273864702</v>
+      </c>
       <c r="AA96" s="26">
         <v>0.186</v>
       </c>
@@ -9944,6 +10265,9 @@
       <c r="Y97" s="24">
         <v>-5.4</v>
       </c>
+      <c r="Z97" s="34">
+        <v>0.45956102013588002</v>
+      </c>
       <c r="AA97" s="26">
         <v>7.1999999999999995E-2</v>
       </c>
@@ -10036,6 +10360,9 @@
       <c r="Y98" s="24">
         <v>-5.6</v>
       </c>
+      <c r="Z98" s="34">
+        <v>-0.29256582260131803</v>
+      </c>
       <c r="AA98" s="26">
         <v>0.04</v>
       </c>
@@ -10134,6 +10461,9 @@
       <c r="Y99" s="24">
         <v>-5.2</v>
       </c>
+      <c r="Z99" s="34">
+        <v>0.577678203582764</v>
+      </c>
       <c r="AA99" s="26">
         <v>7.0000000000000007E-2</v>
       </c>
@@ -10229,6 +10559,9 @@
       <c r="Y100" s="24">
         <v>-4.5999999999999996</v>
       </c>
+      <c r="Z100" s="34">
+        <v>0.332495838403702</v>
+      </c>
       <c r="AA100" s="26">
         <v>5.8000000000000003E-2</v>
       </c>
@@ -10327,6 +10660,9 @@
       <c r="Y101" s="24">
         <v>-4.8</v>
       </c>
+      <c r="Z101" s="34">
+        <v>0.23859010636806499</v>
+      </c>
       <c r="AA101" s="26">
         <v>6.6000000000000003E-2</v>
       </c>
@@ -10422,6 +10758,9 @@
       <c r="Y102" s="24">
         <v>-5</v>
       </c>
+      <c r="Z102" s="34">
+        <v>0.506794452667236</v>
+      </c>
       <c r="AA102" s="26">
         <v>5.8000000000000003E-2</v>
       </c>
@@ -10520,6 +10859,9 @@
       <c r="Y103" s="24">
         <v>-5</v>
       </c>
+      <c r="Z103" s="34">
+        <v>1.04706943035126</v>
+      </c>
       <c r="AA103" s="26">
         <v>0.104</v>
       </c>
@@ -10618,6 +10960,9 @@
       <c r="Y104" s="24">
         <v>-5.2</v>
       </c>
+      <c r="Z104" s="34">
+        <v>0.88112682104110696</v>
+      </c>
       <c r="AA104" s="26">
         <v>0.108</v>
       </c>
@@ -10716,6 +11061,9 @@
       <c r="Y105" s="24">
         <v>-5.4</v>
       </c>
+      <c r="Z105" s="34">
+        <v>0.62847810983657804</v>
+      </c>
       <c r="AA105" s="26">
         <v>0.11600000000000001</v>
       </c>
@@ -10814,6 +11162,9 @@
       <c r="Y106" s="24">
         <v>-4.8</v>
       </c>
+      <c r="Z106" s="34">
+        <v>1.1485115289688099</v>
+      </c>
       <c r="AA106" s="26">
         <v>0.08</v>
       </c>
@@ -10912,6 +11263,9 @@
       <c r="Y107" s="24">
         <v>-4.8</v>
       </c>
+      <c r="Z107" s="34">
+        <v>1.1873749494552599</v>
+      </c>
       <c r="AA107" s="26">
         <v>5.1999999999999998E-2</v>
       </c>
@@ -11010,6 +11364,9 @@
       <c r="Y108" s="24">
         <v>-5</v>
       </c>
+      <c r="Z108" s="34">
+        <v>-3.6042544990777997E-2</v>
+      </c>
       <c r="AA108" s="26">
         <v>0.184</v>
       </c>
@@ -11108,6 +11465,9 @@
       <c r="Y109" s="24">
         <v>-5.4</v>
       </c>
+      <c r="Z109" s="34">
+        <v>-0.44396770000457803</v>
+      </c>
       <c r="AA109" s="26">
         <v>0.122</v>
       </c>
@@ -11206,6 +11566,9 @@
       <c r="Y110" s="24">
         <v>-5.4</v>
       </c>
+      <c r="Z110" s="34">
+        <v>-0.61364668607711803</v>
+      </c>
       <c r="AA110" s="26">
         <v>0.11600000000000001</v>
       </c>
@@ -11301,6 +11664,9 @@
       <c r="Y111" s="24">
         <v>-5.4</v>
       </c>
+      <c r="Z111" s="34">
+        <v>-1.05877757072449</v>
+      </c>
       <c r="AA111" s="26">
         <v>8.7999999999999995E-2</v>
       </c>
@@ -11399,6 +11765,9 @@
       <c r="Y112" s="24">
         <v>-5.8</v>
       </c>
+      <c r="Z112" s="34">
+        <v>0.40498939156532299</v>
+      </c>
       <c r="AA112" s="26">
         <v>7.3999999999999996E-2</v>
       </c>
@@ -11497,6 +11866,9 @@
       <c r="Y113" s="24">
         <v>-5.8</v>
       </c>
+      <c r="Z113" s="34">
+        <v>0.85964542627334595</v>
+      </c>
       <c r="AA113" s="26">
         <v>7.1999999999999995E-2</v>
       </c>
@@ -11595,6 +11967,9 @@
       <c r="Y114" s="24">
         <v>-5</v>
       </c>
+      <c r="Z114" s="34">
+        <v>0.82176518440246604</v>
+      </c>
       <c r="AA114" s="26">
         <v>0.06</v>
       </c>
@@ -11693,6 +12068,9 @@
       <c r="Y115" s="24">
         <v>-5.4</v>
       </c>
+      <c r="Z115" s="34">
+        <v>1.06237256526947</v>
+      </c>
       <c r="AA115" s="26">
         <v>5.3999999999999999E-2</v>
       </c>
@@ -11785,6 +12163,9 @@
       <c r="Y116" s="24">
         <v>-5.6</v>
       </c>
+      <c r="Z116" s="34">
+        <v>0.63910830020904497</v>
+      </c>
       <c r="AA116" s="26">
         <v>0.11600000000000001</v>
       </c>
@@ -11883,6 +12264,9 @@
       <c r="Y117" s="24">
         <v>-5.4</v>
       </c>
+      <c r="Z117" s="34">
+        <v>0.33925038576126099</v>
+      </c>
       <c r="AA117" s="26">
         <v>5.5999999999999999E-3</v>
       </c>
@@ -11981,6 +12365,9 @@
       <c r="Y118" s="24">
         <v>-5.4</v>
       </c>
+      <c r="Z118" s="34">
+        <v>1.10516953468323</v>
+      </c>
       <c r="AA118" s="26">
         <v>8.8000000000000005E-3</v>
       </c>
@@ -12076,6 +12463,9 @@
       <c r="Y119" s="24">
         <v>-5.2</v>
       </c>
+      <c r="Z119" s="34">
+        <v>1.2430517673492401</v>
+      </c>
       <c r="AA119" s="26">
         <v>5.1999999999999998E-3</v>
       </c>
@@ -12174,6 +12564,9 @@
       <c r="Y120" s="24">
         <v>-5</v>
       </c>
+      <c r="Z120" s="34">
+        <v>1.0842412710189799</v>
+      </c>
       <c r="AA120" s="26">
         <v>7.6E-3</v>
       </c>
@@ -12272,6 +12665,9 @@
       <c r="Y121" s="24">
         <v>-4.8</v>
       </c>
+      <c r="Z121" s="34">
+        <v>0.91306573152542103</v>
+      </c>
       <c r="AA121" s="26">
         <v>1.14E-2</v>
       </c>
@@ -12367,6 +12763,9 @@
       <c r="Y122" s="24">
         <v>-5.4</v>
       </c>
+      <c r="Z122" s="34">
+        <v>0.86865139007568404</v>
+      </c>
       <c r="AA122" s="26">
         <v>8.8000000000000005E-3</v>
       </c>
@@ -12465,6 +12864,9 @@
       <c r="Y123" s="24">
         <v>-5.6</v>
       </c>
+      <c r="Z123" s="34">
+        <v>1.01127941161394E-2</v>
+      </c>
       <c r="AA123" s="26">
         <v>7.0000000000000001E-3</v>
       </c>
@@ -12563,6 +12965,9 @@
       <c r="Y124" s="24">
         <v>-5.6</v>
       </c>
+      <c r="Z124" s="34">
+        <v>0.93477457761764504</v>
+      </c>
       <c r="AA124" s="26">
         <v>7.0000000000000001E-3</v>
       </c>
@@ -12661,6 +13066,9 @@
       <c r="Y125" s="24">
         <v>-5.2</v>
       </c>
+      <c r="Z125" s="34">
+        <v>0.68528509140014604</v>
+      </c>
       <c r="AA125" s="26">
         <v>8.3999999999999995E-3</v>
       </c>
@@ -12759,6 +13167,9 @@
       <c r="Y126" s="24">
         <v>-5.2</v>
       </c>
+      <c r="Z126" s="34">
+        <v>-7.2534047067165403E-2</v>
+      </c>
       <c r="AA126" s="26">
         <v>6.6E-3</v>
       </c>
@@ -12857,6 +13268,9 @@
       <c r="Y127" s="24">
         <v>-5.6</v>
       </c>
+      <c r="Z127" s="34">
+        <v>-0.631422638893127</v>
+      </c>
       <c r="AA127" s="26">
         <v>5.0000000000000001E-3</v>
       </c>
@@ -12952,6 +13366,9 @@
       <c r="Y128" s="24">
         <v>-5.4</v>
       </c>
+      <c r="Z128" s="34">
+        <v>-0.33441051840782199</v>
+      </c>
       <c r="AA128" s="26">
         <v>9.4000000000000004E-3</v>
       </c>
@@ -13050,6 +13467,9 @@
       <c r="Y129" s="24">
         <v>-5.4</v>
       </c>
+      <c r="Z129" s="34">
+        <v>-1.4609024524688701</v>
+      </c>
       <c r="AA129" s="26">
         <v>1.84E-2</v>
       </c>
@@ -13145,6 +13565,9 @@
       <c r="Y130" s="24">
         <v>-5.4</v>
       </c>
+      <c r="Z130" s="34">
+        <v>-0.54679387807846103</v>
+      </c>
       <c r="AA130" s="26">
         <v>8.0000000000000002E-3</v>
       </c>
@@ -13243,6 +13666,9 @@
       <c r="Y131" s="24">
         <v>-5.4</v>
       </c>
+      <c r="Z131" s="34">
+        <v>-0.51608967781066895</v>
+      </c>
       <c r="AA131" s="26">
         <v>8.8000000000000005E-3</v>
       </c>
@@ -13338,6 +13764,9 @@
       <c r="Y132" s="24">
         <v>-5.4</v>
       </c>
+      <c r="Z132" s="34">
+        <v>-6.0656785964965799E-2</v>
+      </c>
       <c r="AA132" s="26">
         <v>7.1999999999999998E-3</v>
       </c>
@@ -13433,6 +13862,9 @@
       <c r="Y133" s="24">
         <v>-5.2</v>
       </c>
+      <c r="Z133" s="34">
+        <v>-0.33897441625595098</v>
+      </c>
       <c r="AA133" s="26">
         <v>9.7999999999999997E-3</v>
       </c>
@@ -13528,6 +13960,9 @@
       <c r="Y134" s="24">
         <v>-5.8</v>
       </c>
+      <c r="Z134" s="34">
+        <v>-0.44384598731994601</v>
+      </c>
       <c r="AA134" s="26">
         <v>2.64E-2</v>
       </c>
@@ -13620,6 +14055,9 @@
       <c r="Y135" s="24">
         <v>-5.8</v>
       </c>
+      <c r="Z135" s="34">
+        <v>-0.40992206335067699</v>
+      </c>
       <c r="AA135" s="26">
         <v>1.0800000000000001E-2</v>
       </c>
@@ -13718,6 +14156,9 @@
       <c r="Y136" s="24">
         <v>-5.8</v>
       </c>
+      <c r="Z136" s="34">
+        <v>-0.43029609322547901</v>
+      </c>
       <c r="AA136" s="26">
         <v>1.14E-2</v>
       </c>
@@ -13816,6 +14257,9 @@
       <c r="Y137" s="24">
         <v>-5.2</v>
       </c>
+      <c r="Z137" s="34">
+        <v>0.13664147257804901</v>
+      </c>
       <c r="AA137" s="26">
         <v>1.9400000000000001E-2</v>
       </c>
@@ -13908,6 +14352,9 @@
       <c r="Y138" s="24">
         <v>-4.5999999999999996</v>
       </c>
+      <c r="Z138" s="34">
+        <v>-0.150507152080536</v>
+      </c>
       <c r="AA138" s="26">
         <v>4.6600000000000003E-2</v>
       </c>
@@ -14003,6 +14450,9 @@
       <c r="Y139" s="24">
         <v>-4.5999999999999996</v>
       </c>
+      <c r="Z139" s="34">
+        <v>-0.32785838842392001</v>
+      </c>
       <c r="AA139" s="26">
         <v>4.3400000000000001E-2</v>
       </c>
@@ -14098,6 +14548,9 @@
       <c r="Y140" s="24">
         <v>-4.5999999999999996</v>
       </c>
+      <c r="Z140" s="34">
+        <v>-0.81611645221710205</v>
+      </c>
       <c r="AA140" s="26">
         <v>4.36E-2</v>
       </c>
@@ -14193,6 +14646,9 @@
       <c r="Y141" s="24">
         <v>-5</v>
       </c>
+      <c r="Z141" s="34">
+        <v>-0.67411023378372203</v>
+      </c>
       <c r="AA141" s="26">
         <v>4.6800000000000001E-2</v>
       </c>
@@ -14291,6 +14747,9 @@
       <c r="Y142" s="24">
         <v>-5.8</v>
       </c>
+      <c r="Z142" s="34">
+        <v>-0.43447366356849698</v>
+      </c>
       <c r="AA142" s="26">
         <v>4.5400000000000003E-2</v>
       </c>
@@ -14389,6 +14848,9 @@
       <c r="Y143" s="24">
         <v>-5.6</v>
       </c>
+      <c r="Z143" s="34">
+        <v>-0.45780172944068898</v>
+      </c>
       <c r="AA143" s="26">
         <v>5.1999999999999998E-2</v>
       </c>
@@ -14487,6 +14949,9 @@
       <c r="Y144" s="24">
         <v>-5.6</v>
       </c>
+      <c r="Z144" s="34">
+        <v>-0.64707946777343806</v>
+      </c>
       <c r="AA144" s="26">
         <v>5.7200000000000001E-2</v>
       </c>
@@ -14585,6 +15050,9 @@
       <c r="Y145" s="24">
         <v>-5.8</v>
       </c>
+      <c r="Z145" s="34">
+        <v>-0.185409426689148</v>
+      </c>
       <c r="AA145" s="26">
         <v>3.7400000000000003E-2</v>
       </c>
@@ -14680,6 +15148,9 @@
       <c r="Y146" s="24">
         <v>-6.2</v>
       </c>
+      <c r="Z146" s="34">
+        <v>-1.1557304859161399</v>
+      </c>
       <c r="AA146" s="26">
         <v>3.2199999999999999E-2</v>
       </c>
@@ -14778,6 +15249,9 @@
       <c r="Y147" s="24">
         <v>-6.2</v>
       </c>
+      <c r="Z147" s="34">
+        <v>-2.4332856759428999E-2</v>
+      </c>
       <c r="AA147" s="26">
         <v>3.3000000000000002E-2</v>
       </c>
@@ -14876,6 +15350,9 @@
       <c r="Y148" s="24">
         <v>-6.2</v>
       </c>
+      <c r="Z148" s="34">
+        <v>-0.39858931303024298</v>
+      </c>
       <c r="AA148" s="26">
         <v>3.32E-2</v>
       </c>
@@ -14974,6 +15451,9 @@
       <c r="Y149" s="24">
         <v>-6.2</v>
       </c>
+      <c r="Z149" s="34">
+        <v>-0.12667325139045699</v>
+      </c>
       <c r="AA149" s="26">
         <v>3.6400000000000002E-2</v>
       </c>
@@ -15069,6 +15549,9 @@
       <c r="Y150" s="24">
         <v>-5.8</v>
       </c>
+      <c r="Z150" s="34">
+        <v>-0.22955544292926799</v>
+      </c>
       <c r="AA150" s="26">
         <v>4.4400000000000002E-2</v>
       </c>
@@ -15167,6 +15650,9 @@
       <c r="Y151" s="24">
         <v>-6</v>
       </c>
+      <c r="Z151" s="34">
+        <v>0.29305428266525302</v>
+      </c>
       <c r="AA151" s="26">
         <v>4.1399999999999999E-2</v>
       </c>
@@ -15265,6 +15751,9 @@
       <c r="Y152" s="24">
         <v>-6</v>
       </c>
+      <c r="Z152" s="34">
+        <v>0.46575871109962502</v>
+      </c>
       <c r="AA152" s="26">
         <v>4.1399999999999999E-2</v>
       </c>
@@ -15363,6 +15852,9 @@
       <c r="Y153" s="24">
         <v>-5.6</v>
       </c>
+      <c r="Z153" s="34">
+        <v>0.46970382332801802</v>
+      </c>
       <c r="AA153" s="26">
         <v>3.7199999999999997E-2</v>
       </c>
@@ -15461,6 +15953,9 @@
       <c r="Y154" s="24">
         <v>-5.2</v>
       </c>
+      <c r="Z154" s="34">
+        <v>-0.192948713898659</v>
+      </c>
       <c r="AA154" s="26">
         <v>3.4000000000000002E-2</v>
       </c>
@@ -15559,6 +16054,9 @@
       <c r="Y155" s="24">
         <v>-5.6</v>
       </c>
+      <c r="Z155" s="34">
+        <v>0.84724551439285301</v>
+      </c>
       <c r="AA155" s="26">
         <v>3.2800000000000003E-2</v>
       </c>
@@ -15657,6 +16155,9 @@
       <c r="Y156" s="24">
         <v>-5.4</v>
       </c>
+      <c r="Z156" s="34">
+        <v>-0.48054862022399902</v>
+      </c>
       <c r="AA156" s="26">
         <v>3.3599999999999998E-2</v>
       </c>
@@ -15755,6 +16256,9 @@
       <c r="Y157" s="24">
         <v>-5.4</v>
       </c>
+      <c r="Z157" s="34">
+        <v>-0.55028527975082397</v>
+      </c>
       <c r="AA157" s="26">
         <v>3.2399999999999998E-2</v>
       </c>
@@ -15853,6 +16357,9 @@
       <c r="Y158" s="24">
         <v>-5.4</v>
       </c>
+      <c r="Z158" s="34">
+        <v>-0.25257301330566401</v>
+      </c>
       <c r="AA158" s="26">
         <v>3.6799999999999999E-2</v>
       </c>
@@ -15951,6 +16458,9 @@
       <c r="Y159" s="24">
         <v>-5.4</v>
       </c>
+      <c r="Z159" s="34">
+        <v>-0.11767870187759399</v>
+      </c>
       <c r="AA159" s="26">
         <v>2.9399999999999999E-2</v>
       </c>
@@ -16049,6 +16559,9 @@
       <c r="Y160" s="24">
         <v>-5.4</v>
       </c>
+      <c r="Z160" s="34">
+        <v>-7.5633637607097598E-2</v>
+      </c>
       <c r="AA160" s="26">
         <v>3.04E-2</v>
       </c>
@@ -16147,6 +16660,9 @@
       <c r="Y161" s="24">
         <v>-5.4</v>
       </c>
+      <c r="Z161" s="34">
+        <v>0.10595990717411</v>
+      </c>
       <c r="AA161" s="26">
         <v>4.4400000000000002E-2</v>
       </c>
@@ -16242,6 +16758,9 @@
       <c r="Y162" s="24">
         <v>-4.8</v>
       </c>
+      <c r="Z162" s="34">
+        <v>0.275389194488525</v>
+      </c>
       <c r="AA162" s="26">
         <v>3.8399999999999997E-2</v>
       </c>
@@ -16337,6 +16856,9 @@
       <c r="Y163" s="24">
         <v>-5.2</v>
       </c>
+      <c r="Z163" s="34">
+        <v>0.51226061582565297</v>
+      </c>
       <c r="AA163" s="26">
         <v>3.0599999999999999E-2</v>
       </c>
@@ -16435,6 +16957,9 @@
       <c r="Y164" s="24">
         <v>-5.2</v>
       </c>
+      <c r="Z164" s="34">
+        <v>0.113179244101048</v>
+      </c>
       <c r="AA164" s="26">
         <v>3.44E-2</v>
       </c>
@@ -16533,6 +17058,9 @@
       <c r="Y165" s="24">
         <v>-5</v>
       </c>
+      <c r="Z165" s="34">
+        <v>0.61989295482635498</v>
+      </c>
       <c r="AA165" s="26">
         <v>3.32E-2</v>
       </c>
@@ -16631,6 +17159,9 @@
       <c r="Y166" s="24">
         <v>-5</v>
       </c>
+      <c r="Z166" s="34">
+        <v>0.46221321821212802</v>
+      </c>
       <c r="AA166" s="26">
         <v>3.3399999999999999E-2</v>
       </c>
@@ -16726,6 +17257,9 @@
       <c r="Y167" s="24">
         <v>-5.2</v>
       </c>
+      <c r="Z167" s="34">
+        <v>-5.2351549267768901E-2</v>
+      </c>
       <c r="AA167" s="26">
         <v>3.1199999999999999E-2</v>
       </c>
@@ -16821,6 +17355,9 @@
       <c r="Y168" s="24">
         <v>-5</v>
       </c>
+      <c r="Z168" s="34">
+        <v>-0.31811860203742998</v>
+      </c>
       <c r="AA168" s="26">
         <v>0.03</v>
       </c>
@@ -16919,6 +17456,9 @@
       <c r="Y169" s="24">
         <v>-5.8</v>
       </c>
+      <c r="Z169" s="34">
+        <v>1.3989384174346899</v>
+      </c>
       <c r="AA169" s="26">
         <v>2.8000000000000001E-2</v>
       </c>
@@ -17017,6 +17557,9 @@
       <c r="Y170" s="24">
         <v>-6</v>
       </c>
+      <c r="Z170" s="34">
+        <v>0.62627881765365601</v>
+      </c>
       <c r="AA170" s="26">
         <v>2.9000000000000001E-2</v>
       </c>
@@ -17115,6 +17658,9 @@
       <c r="Y171" s="24">
         <v>-5.6</v>
       </c>
+      <c r="Z171" s="34">
+        <v>1.5982463359832799</v>
+      </c>
       <c r="AA171" s="26">
         <v>3.7999999999999999E-2</v>
       </c>
@@ -17210,6 +17756,9 @@
       <c r="Y172" s="24">
         <v>-5.4</v>
       </c>
+      <c r="Z172" s="34">
+        <v>-0.44187805056571999</v>
+      </c>
       <c r="AA172" s="26">
         <v>5.7000000000000002E-2</v>
       </c>
@@ -17305,6 +17854,9 @@
       <c r="Y173" s="24">
         <v>-5.2</v>
       </c>
+      <c r="Z173" s="34">
+        <v>-0.30543339252471902</v>
+      </c>
       <c r="AA173" s="26">
         <v>3.5200000000000002E-2</v>
       </c>
@@ -17403,6 +17955,9 @@
       <c r="Y174" s="24">
         <v>-5.4</v>
       </c>
+      <c r="Z174" s="34">
+        <v>-1.6074798107147199</v>
+      </c>
       <c r="AA174" s="26">
         <v>2.92E-2</v>
       </c>
@@ -17501,6 +18056,9 @@
       <c r="Y175" s="24">
         <v>-5.4</v>
       </c>
+      <c r="Z175" s="34">
+        <v>-0.248051062226295</v>
+      </c>
       <c r="AA175" s="26">
         <v>3.7999999999999999E-2</v>
       </c>
@@ -17599,6 +18157,9 @@
       <c r="Y176" s="24">
         <v>-5.4</v>
       </c>
+      <c r="Z176" s="34">
+        <v>-0.34316942095756497</v>
+      </c>
       <c r="AA176" s="26">
         <v>3.7999999999999999E-2</v>
       </c>
@@ -17697,6 +18258,9 @@
       <c r="Y177" s="24">
         <v>-5.4</v>
       </c>
+      <c r="Z177" s="34">
+        <v>-0.26575478911399802</v>
+      </c>
       <c r="AA177" s="26">
         <v>3.3000000000000002E-2</v>
       </c>
@@ -17795,6 +18359,9 @@
       <c r="Y178" s="24">
         <v>-5.4</v>
       </c>
+      <c r="Z178" s="34">
+        <v>-0.75576674938201904</v>
+      </c>
       <c r="AA178" s="26">
         <v>3.4599999999999999E-2</v>
       </c>
@@ -17893,6 +18460,9 @@
       <c r="Y179" s="24">
         <v>-5.2</v>
       </c>
+      <c r="Z179" s="34">
+        <v>-0.57919496297836304</v>
+      </c>
       <c r="AA179" s="26">
         <v>3.3799999999999997E-2</v>
       </c>
@@ -17988,6 +18558,9 @@
       <c r="Y180" s="24">
         <v>-5</v>
       </c>
+      <c r="Z180" s="34">
+        <v>-0.93849760293960605</v>
+      </c>
       <c r="AA180" s="26">
         <v>3.0599999999999999E-2</v>
       </c>
@@ -18086,6 +18659,9 @@
       <c r="Y181" s="24">
         <v>-5</v>
       </c>
+      <c r="Z181" s="34">
+        <v>-0.559922695159912</v>
+      </c>
       <c r="AA181" s="26">
         <v>3.3599999999999998E-2</v>
       </c>
@@ -18184,6 +18760,9 @@
       <c r="Y182" s="24">
         <v>-5</v>
       </c>
+      <c r="Z182" s="34">
+        <v>-0.52611517906188998</v>
+      </c>
       <c r="AA182" s="26">
         <v>4.5199999999999997E-2</v>
       </c>
@@ -18282,6 +18861,9 @@
       <c r="Y183" s="24">
         <v>-5</v>
       </c>
+      <c r="Z183" s="34">
+        <v>-2.8207832947373399E-3</v>
+      </c>
       <c r="AA183" s="26">
         <v>3.1800000000000002E-2</v>
       </c>
@@ -18380,6 +18962,9 @@
       <c r="Y184" s="24">
         <v>-5.2</v>
       </c>
+      <c r="Z184" s="34">
+        <v>-0.15357121825218201</v>
+      </c>
       <c r="AA184" s="26">
         <v>3.1600000000000003E-2</v>
       </c>
@@ -18478,6 +19063,9 @@
       <c r="Y185" s="24">
         <v>-5.2</v>
       </c>
+      <c r="Z185" s="34">
+        <v>-0.182380571961403</v>
+      </c>
       <c r="AA185" s="26">
         <v>3.9600000000000003E-2</v>
       </c>
@@ -18573,6 +19161,9 @@
       <c r="Y186" s="24">
         <v>-5.2</v>
       </c>
+      <c r="Z186" s="34">
+        <v>-0.21023927628993999</v>
+      </c>
       <c r="AA186" s="26">
         <v>3.0800000000000001E-2</v>
       </c>
@@ -18671,6 +19262,9 @@
       <c r="Y187" s="24">
         <v>-5.6</v>
       </c>
+      <c r="Z187" s="34">
+        <v>-1.6251969337463399</v>
+      </c>
       <c r="AA187" s="26">
         <v>0.03</v>
       </c>
@@ -18769,6 +19363,9 @@
       <c r="Y188" s="24">
         <v>-5.4</v>
       </c>
+      <c r="Z188" s="34">
+        <v>-1.0913952589035001</v>
+      </c>
       <c r="AA188" s="26">
         <v>3.5799999999999998E-2</v>
       </c>
@@ -18867,6 +19464,9 @@
       <c r="Y189" s="24">
         <v>-5.2</v>
       </c>
+      <c r="Z189" s="34">
+        <v>-0.25164783000946001</v>
+      </c>
       <c r="AA189" s="26">
         <v>5.5599999999999997E-2</v>
       </c>
@@ -18965,6 +19565,9 @@
       <c r="Y190" s="24">
         <v>-5.6</v>
       </c>
+      <c r="Z190" s="34">
+        <v>-0.66141092777252197</v>
+      </c>
       <c r="AA190" s="26">
         <v>3.8199999999999998E-2</v>
       </c>
@@ -19063,6 +19666,9 @@
       <c r="Y191" s="24">
         <v>-5.8</v>
       </c>
+      <c r="Z191" s="34">
+        <v>-1.33437812328339</v>
+      </c>
       <c r="AA191" s="26">
         <v>3.6799999999999999E-2</v>
       </c>
@@ -19161,6 +19767,9 @@
       <c r="Y192" s="24">
         <v>-5.4</v>
       </c>
+      <c r="Z192" s="34">
+        <v>-0.970264732837677</v>
+      </c>
       <c r="AA192" s="26">
         <v>4.1200000000000001E-2</v>
       </c>
@@ -19259,6 +19868,9 @@
       <c r="Y193" s="24">
         <v>-5.2</v>
       </c>
+      <c r="Z193" s="34">
+        <v>3.50908446125686E-3</v>
+      </c>
       <c r="AA193" s="26">
         <v>3.1800000000000002E-2</v>
       </c>
@@ -19357,6 +19969,9 @@
       <c r="Y194" s="24">
         <v>-5</v>
       </c>
+      <c r="Z194" s="34">
+        <v>-0.30824753642082198</v>
+      </c>
       <c r="AA194" s="26">
         <v>4.7600000000000003E-2</v>
       </c>
@@ -19452,6 +20067,9 @@
       <c r="Y195" s="24">
         <v>-5.8</v>
       </c>
+      <c r="Z195" s="34">
+        <v>0.13461755216121701</v>
+      </c>
       <c r="AA195" s="26">
         <v>5.04E-2</v>
       </c>
@@ -19550,6 +20168,9 @@
       <c r="Y196" s="24">
         <v>-5.6</v>
       </c>
+      <c r="Z196" s="34">
+        <v>-0.48978269100189198</v>
+      </c>
       <c r="AA196" s="26">
         <v>3.32E-2</v>
       </c>
@@ -19648,6 +20269,9 @@
       <c r="Y197" s="24">
         <v>-5.8</v>
       </c>
+      <c r="Z197" s="34">
+        <v>-1.6693478822708101</v>
+      </c>
       <c r="AA197" s="26">
         <v>3.2599999999999997E-2</v>
       </c>
@@ -19746,6 +20370,9 @@
       <c r="Y198" s="24">
         <v>-5.4</v>
       </c>
+      <c r="Z198" s="34">
+        <v>-1.6353286504745499</v>
+      </c>
       <c r="AA198" s="26">
         <v>3.4200000000000001E-2</v>
       </c>
@@ -19844,6 +20471,9 @@
       <c r="Y199" s="24">
         <v>-5.2</v>
       </c>
+      <c r="Z199" s="34">
+        <v>-1.9870907068252599</v>
+      </c>
       <c r="AA199" s="26">
         <v>3.3799999999999997E-2</v>
       </c>
@@ -19942,6 +20572,9 @@
       <c r="Y200" s="24">
         <v>-5.4</v>
       </c>
+      <c r="Z200" s="34">
+        <v>-2.08388328552246</v>
+      </c>
       <c r="AA200" s="26">
         <v>4.3400000000000001E-2</v>
       </c>
@@ -20040,6 +20673,9 @@
       <c r="Y201" s="24">
         <v>-5.2</v>
       </c>
+      <c r="Z201" s="34">
+        <v>-0.60965162515640303</v>
+      </c>
       <c r="AA201" s="26">
         <v>4.2799999999999998E-2</v>
       </c>
@@ -20138,6 +20774,9 @@
       <c r="Y202" s="24">
         <v>-5.4</v>
       </c>
+      <c r="Z202" s="34">
+        <v>-0.74442446231841997</v>
+      </c>
       <c r="AA202" s="26">
         <v>5.2999999999999999E-2</v>
       </c>
@@ -20236,6 +20875,9 @@
       <c r="Y203" s="24">
         <v>-5.6</v>
       </c>
+      <c r="Z203" s="34">
+        <v>-0.764712274074554</v>
+      </c>
       <c r="AA203" s="26">
         <v>0.04</v>
       </c>
@@ -20331,6 +20973,9 @@
       <c r="Y204" s="24">
         <v>-6</v>
       </c>
+      <c r="Z204" s="34">
+        <v>-0.27636468410491899</v>
+      </c>
       <c r="AA204" s="26">
         <v>5.3600000000000002E-2</v>
       </c>
@@ -20429,6 +21074,9 @@
       <c r="Y205" s="24">
         <v>-6.2</v>
       </c>
+      <c r="Z205" s="34">
+        <v>-1.18121898174286</v>
+      </c>
       <c r="AA205" s="26">
         <v>3.04E-2</v>
       </c>
@@ -20527,6 +21175,9 @@
       <c r="Y206" s="24">
         <v>-6.2</v>
       </c>
+      <c r="Z206" s="34">
+        <v>-1.0472786426544201</v>
+      </c>
       <c r="AA206" s="26">
         <v>3.0599999999999999E-2</v>
       </c>
@@ -20625,6 +21276,9 @@
       <c r="Y207" s="24">
         <v>-6.4</v>
       </c>
+      <c r="Z207" s="34">
+        <v>-0.20155368745326999</v>
+      </c>
       <c r="AA207" s="26">
         <v>3.1199999999999999E-2</v>
       </c>
@@ -20723,6 +21377,9 @@
       <c r="Y208" s="24">
         <v>-6.4</v>
       </c>
+      <c r="Z208" s="34">
+        <v>-0.23126807808875999</v>
+      </c>
       <c r="AA208" s="26">
         <v>3.2199999999999999E-2</v>
       </c>
@@ -20818,6 +21475,9 @@
       <c r="Y209" s="24">
         <v>-5.4</v>
       </c>
+      <c r="Z209" s="34">
+        <v>-0.52136647701263406</v>
+      </c>
       <c r="AA209" s="26">
         <v>4.8399999999999999E-2</v>
       </c>
@@ -20913,6 +21573,9 @@
       <c r="Y210" s="24">
         <v>-5.8</v>
       </c>
+      <c r="Z210" s="34">
+        <v>-0.42980107665062001</v>
+      </c>
       <c r="AA210" s="26">
         <v>4.8599999999999997E-2</v>
       </c>
@@ -21008,6 +21671,9 @@
       <c r="Y211" s="24">
         <v>-5.8</v>
       </c>
+      <c r="Z211" s="34">
+        <v>-2.1146337985992401</v>
+      </c>
       <c r="AA211" s="26">
         <v>3.4799999999999998E-2</v>
       </c>
@@ -21106,6 +21772,9 @@
       <c r="Y212" s="24">
         <v>-5.6</v>
       </c>
+      <c r="Z212" s="34">
+        <v>-1.36216151714325</v>
+      </c>
       <c r="AA212" s="26">
         <v>4.5999999999999999E-2</v>
       </c>
@@ -21204,6 +21873,9 @@
       <c r="Y213" s="24">
         <v>-5.8</v>
       </c>
+      <c r="Z213" s="34">
+        <v>-1.1857317686080899</v>
+      </c>
       <c r="AA213" s="26">
         <v>3.5799999999999998E-2</v>
       </c>
@@ -21302,6 +21974,9 @@
       <c r="Y214" s="24">
         <v>-6</v>
       </c>
+      <c r="Z214" s="34">
+        <v>-0.809728503227234</v>
+      </c>
       <c r="AA214" s="26">
         <v>3.2599999999999997E-2</v>
       </c>
@@ -21400,6 +22075,9 @@
       <c r="Y215" s="24">
         <v>-5.8</v>
       </c>
+      <c r="Z215" s="34">
+        <v>-0.65047276020050004</v>
+      </c>
       <c r="AA215" s="26">
         <v>1.5800000000000002E-2</v>
       </c>
@@ -21498,6 +22176,9 @@
       <c r="Y216" s="24">
         <v>-5.6</v>
       </c>
+      <c r="Z216" s="34">
+        <v>-0.83348941802978505</v>
+      </c>
       <c r="AA216" s="26">
         <v>1.14E-2</v>
       </c>
@@ -21596,6 +22277,9 @@
       <c r="Y217" s="24">
         <v>-5.6</v>
       </c>
+      <c r="Z217" s="34">
+        <v>-0.59808683395385698</v>
+      </c>
       <c r="AA217" s="26">
         <v>0.03</v>
       </c>
@@ -21694,6 +22378,9 @@
       <c r="Y218" s="24">
         <v>-5.8</v>
       </c>
+      <c r="Z218" s="34">
+        <v>-1.4505876302719101</v>
+      </c>
       <c r="AA218" s="26">
         <v>2.5999999999999999E-3</v>
       </c>
@@ -21792,6 +22479,9 @@
       <c r="Y219" s="24">
         <v>-5.4</v>
       </c>
+      <c r="Z219" s="34">
+        <v>-1.1535074710845901</v>
+      </c>
       <c r="AA219" s="26">
         <v>4.7999999999999996E-3</v>
       </c>
@@ -21890,6 +22580,9 @@
       <c r="Y220" s="24">
         <v>-5</v>
       </c>
+      <c r="Z220" s="34">
+        <v>-0.318503618240356</v>
+      </c>
       <c r="AA220" s="26">
         <v>8.9999999999999993E-3</v>
       </c>
@@ -21988,6 +22681,9 @@
       <c r="Y221" s="24">
         <v>-5.6</v>
       </c>
+      <c r="Z221" s="34">
+        <v>-0.14182026684284199</v>
+      </c>
       <c r="AA221" s="26">
         <v>9.4000000000000004E-3</v>
       </c>
@@ -22086,6 +22782,9 @@
       <c r="Y222" s="24">
         <v>-5.8</v>
       </c>
+      <c r="Z222" s="34">
+        <v>-0.54390060901641801</v>
+      </c>
       <c r="AA222" s="26">
         <v>2.5999999999999999E-3</v>
       </c>
@@ -22184,6 +22883,9 @@
       <c r="Y223" s="24">
         <v>-5.8</v>
       </c>
+      <c r="Z223" s="34">
+        <v>-0.333393543958664</v>
+      </c>
       <c r="AA223" s="26">
         <v>2.5999999999999999E-3</v>
       </c>
@@ -22282,6 +22984,9 @@
       <c r="Y224" s="24">
         <v>-5.6</v>
       </c>
+      <c r="Z224" s="34">
+        <v>-0.42736929655075101</v>
+      </c>
       <c r="AA224" s="26">
         <v>2.5999999999999999E-3</v>
       </c>
@@ -22380,6 +23085,9 @@
       <c r="Y225" s="24">
         <v>-5.6</v>
       </c>
+      <c r="Z225" s="34">
+        <v>-0.47888475656509399</v>
+      </c>
       <c r="AA225" s="26">
         <v>2.5999999999999999E-3</v>
       </c>
@@ -22478,6 +23186,9 @@
       <c r="Y226" s="24">
         <v>-5.6</v>
       </c>
+      <c r="Z226" s="34">
+        <v>0.14740440249443101</v>
+      </c>
       <c r="AA226" s="26">
         <v>1.54E-2</v>
       </c>
@@ -22576,6 +23287,9 @@
       <c r="Y227" s="24">
         <v>-5.6</v>
       </c>
+      <c r="Z227" s="34">
+        <v>-0.62584471702575695</v>
+      </c>
       <c r="AA227" s="26">
         <v>6.6E-3</v>
       </c>
@@ -22668,6 +23382,9 @@
       <c r="Y228" s="24">
         <v>-5.2</v>
       </c>
+      <c r="Z228" s="34">
+        <v>-0.47670981287956199</v>
+      </c>
       <c r="AA228" s="26">
         <v>3.5999999999999999E-3</v>
       </c>
@@ -22766,6 +23483,9 @@
       <c r="Y229" s="24">
         <v>-5.2</v>
       </c>
+      <c r="Z229" s="34">
+        <v>-0.79288971424102805</v>
+      </c>
       <c r="AA229" s="26">
         <v>4.7999999999999996E-3</v>
       </c>
@@ -22864,6 +23584,9 @@
       <c r="Y230" s="24">
         <v>-5.4</v>
       </c>
+      <c r="Z230" s="34">
+        <v>-0.59754157066345204</v>
+      </c>
       <c r="AA230" s="26">
         <v>2.5999999999999999E-3</v>
       </c>
@@ -22962,6 +23685,9 @@
       <c r="Y231" s="24">
         <v>-5.4</v>
       </c>
+      <c r="Z231" s="34">
+        <v>-0.63715749979019198</v>
+      </c>
       <c r="AA231" s="26">
         <v>2.5999999999999999E-3</v>
       </c>
@@ -23060,6 +23786,9 @@
       <c r="Y232" s="24">
         <v>-5.2</v>
       </c>
+      <c r="Z232" s="34">
+        <v>-0.25585010647773698</v>
+      </c>
       <c r="AA232" s="26">
         <v>2.5999999999999999E-3</v>
       </c>
@@ -23155,6 +23884,9 @@
       <c r="Y233" s="24">
         <v>-5.2</v>
       </c>
+      <c r="Z233" s="34">
+        <v>-0.68538200855255105</v>
+      </c>
       <c r="AA233" s="26">
         <v>1.9599999999999999E-2</v>
       </c>
@@ -23253,6 +23985,9 @@
       <c r="Y234" s="24">
         <v>-5</v>
       </c>
+      <c r="Z234" s="34">
+        <v>-0.387709081172943</v>
+      </c>
       <c r="AA234" s="26">
         <v>2.3E-2</v>
       </c>
@@ -23351,6 +24086,9 @@
       <c r="Y235" s="24">
         <v>-5.4</v>
       </c>
+      <c r="Z235" s="34">
+        <v>0.36118751764297502</v>
+      </c>
       <c r="AA235" s="26">
         <v>2.18E-2</v>
       </c>
@@ -23449,6 +24187,9 @@
       <c r="Y236" s="24">
         <v>-5.6</v>
       </c>
+      <c r="Z236" s="34">
+        <v>0.26393890380859403</v>
+      </c>
       <c r="AA236" s="26">
         <v>2.8199999999999999E-2</v>
       </c>
@@ -23544,6 +24285,9 @@
       <c r="Y237" s="24">
         <v>-5</v>
       </c>
+      <c r="Z237" s="34">
+        <v>-0.35544082522392301</v>
+      </c>
       <c r="AA237" s="26">
         <v>1.66E-2</v>
       </c>
@@ -23642,6 +24386,9 @@
       <c r="Y238" s="24">
         <v>-5.4</v>
       </c>
+      <c r="Z238" s="34">
+        <v>0.21044665575027499</v>
+      </c>
       <c r="AA238" s="26">
         <v>1.6199999999999999E-2</v>
       </c>
@@ -23740,6 +24487,9 @@
       <c r="Y239" s="24">
         <v>-5.8</v>
       </c>
+      <c r="Z239" s="34">
+        <v>0.60484284162521396</v>
+      </c>
       <c r="AA239" s="26">
         <v>1.26E-2</v>
       </c>
@@ -23838,6 +24588,9 @@
       <c r="Y240" s="24">
         <v>-5.6</v>
       </c>
+      <c r="Z240" s="34">
+        <v>-0.44881168007850603</v>
+      </c>
       <c r="AA240" s="26">
         <v>1.0200000000000001E-2</v>
       </c>
@@ -23936,6 +24689,9 @@
       <c r="Y241" s="24">
         <v>-5.6</v>
       </c>
+      <c r="Z241" s="34">
+        <v>-0.35206082463264499</v>
+      </c>
       <c r="AA241" s="26">
         <v>1.0800000000000001E-2</v>
       </c>
@@ -24034,6 +24790,9 @@
       <c r="Y242" s="24">
         <v>-5.2</v>
       </c>
+      <c r="Z242" s="34">
+        <v>-0.48946908116340598</v>
+      </c>
       <c r="AA242" s="26">
         <v>1.24E-2</v>
       </c>
@@ -24132,6 +24891,9 @@
       <c r="Y243" s="24">
         <v>-5.4</v>
       </c>
+      <c r="Z243" s="34">
+        <v>0.18431466817855799</v>
+      </c>
       <c r="AA243" s="26">
         <v>9.5999999999999992E-3</v>
       </c>
@@ -24227,6 +24989,9 @@
       <c r="Y244" s="24">
         <v>-5.4</v>
       </c>
+      <c r="Z244" s="34">
+        <v>-0.71863216161727905</v>
+      </c>
       <c r="AA244" s="26">
         <v>2.92E-2</v>
       </c>
@@ -24325,6 +25090,9 @@
       <c r="Y245" s="24">
         <v>-5</v>
       </c>
+      <c r="Z245" s="34">
+        <v>0.14315828680992099</v>
+      </c>
       <c r="AA245" s="26">
         <v>1.18E-2</v>
       </c>
@@ -24423,6 +25191,9 @@
       <c r="Y246" s="24">
         <v>-4.8</v>
       </c>
+      <c r="Z246" s="34">
+        <v>-0.89712888002395597</v>
+      </c>
       <c r="AA246" s="26">
         <v>4.1999999999999997E-3</v>
       </c>
@@ -24521,6 +25292,9 @@
       <c r="Y247" s="24">
         <v>-4.8</v>
       </c>
+      <c r="Z247" s="34">
+        <v>-0.67631989717483498</v>
+      </c>
       <c r="AA247" s="26">
         <v>6.1999999999999998E-3</v>
       </c>
@@ -24619,6 +25393,9 @@
       <c r="Y248" s="24">
         <v>-4.8</v>
       </c>
+      <c r="Z248" s="34">
+        <v>-0.77528393268585205</v>
+      </c>
       <c r="AA248" s="26">
         <v>2.3999999999999998E-3</v>
       </c>
@@ -24717,6 +25494,9 @@
       <c r="Y249" s="24">
         <v>-5.2</v>
       </c>
+      <c r="Z249" s="34">
+        <v>4.3042410165071501E-2</v>
+      </c>
       <c r="AA249" s="26">
         <v>2.3999999999999998E-3</v>
       </c>
@@ -24809,6 +25589,9 @@
       <c r="Y250" s="24">
         <v>-5.8</v>
       </c>
+      <c r="Z250" s="34">
+        <v>0.14386779069900499</v>
+      </c>
       <c r="AA250" s="26">
         <v>2.5999999999999999E-3</v>
       </c>
@@ -24907,6 +25690,9 @@
       <c r="Y251" s="24">
         <v>-6</v>
       </c>
+      <c r="Z251" s="34">
+        <v>-0.320410877466202</v>
+      </c>
       <c r="AA251" s="26">
         <v>2.5999999999999999E-3</v>
       </c>
@@ -25002,6 +25788,9 @@
       <c r="Y252" s="24">
         <v>-5</v>
       </c>
+      <c r="Z252" s="34">
+        <v>-0.101104460656643</v>
+      </c>
       <c r="AA252" s="26">
         <v>2.5999999999999999E-3</v>
       </c>
@@ -25100,6 +25889,9 @@
       <c r="Y253" s="24">
         <v>-5</v>
       </c>
+      <c r="Z253" s="34">
+        <v>-0.62908303737640403</v>
+      </c>
       <c r="AA253" s="26">
         <v>6.0000000000000001E-3</v>
       </c>
@@ -25192,6 +25984,9 @@
       <c r="Y254" s="24">
         <v>-4.8</v>
       </c>
+      <c r="Z254" s="34">
+        <v>-0.27308186888694802</v>
+      </c>
       <c r="AA254" s="26">
         <v>1.9599999999999999E-2</v>
       </c>
@@ -25290,6 +26085,9 @@
       <c r="Y255" s="24">
         <v>-4.5999999999999996</v>
       </c>
+      <c r="Z255" s="34">
+        <v>0.170166611671448</v>
+      </c>
       <c r="AA255" s="26">
         <v>4.7600000000000003E-2</v>
       </c>
@@ -25388,6 +26186,9 @@
       <c r="Y256" s="24">
         <v>-4.8</v>
       </c>
+      <c r="Z256" s="34">
+        <v>-5.70246167480946E-2</v>
+      </c>
       <c r="AA256" s="26">
         <v>1.3599999999999999E-2</v>
       </c>
@@ -25468,6 +26269,9 @@
       <c r="Y257" s="24">
         <v>-4.5999999999999996</v>
       </c>
+      <c r="Z257" s="34">
+        <v>-0.60603046417236295</v>
+      </c>
       <c r="AA257" s="26">
         <v>1.0999999999999999E-2</v>
       </c>
@@ -25557,6 +26361,9 @@
       <c r="Y258" s="24">
         <v>-5.2</v>
       </c>
+      <c r="Z258" s="34">
+        <v>-0.27984529733657798</v>
+      </c>
       <c r="AA258" s="26">
         <v>2.8199999999999999E-2</v>
       </c>
@@ -25655,6 +26462,9 @@
       <c r="Y259" s="24">
         <v>-6</v>
       </c>
+      <c r="Z259" s="34">
+        <v>0.80029875040054299</v>
+      </c>
       <c r="AA259" s="26">
         <v>1.4800000000000001E-2</v>
       </c>
@@ -25753,6 +26563,9 @@
       <c r="Y260" s="24">
         <v>-5.6</v>
       </c>
+      <c r="Z260" s="34">
+        <v>-7.3093943297863007E-2</v>
+      </c>
       <c r="AA260" s="26">
         <v>1.0800000000000001E-2</v>
       </c>
@@ -25851,6 +26664,9 @@
       <c r="Y261" s="24">
         <v>-5.8</v>
       </c>
+      <c r="Z261" s="34">
+        <v>0.60211062431335405</v>
+      </c>
       <c r="AA261" s="26">
         <v>2.5999999999999999E-3</v>
       </c>
@@ -25949,6 +26765,9 @@
       <c r="Y262" s="24">
         <v>-5.8</v>
       </c>
+      <c r="Z262" s="34">
+        <v>0.31759276986122098</v>
+      </c>
       <c r="AA262" s="26">
         <v>2.5999999999999999E-3</v>
       </c>
@@ -26047,6 +26866,9 @@
       <c r="Y263" s="24">
         <v>-5.8</v>
       </c>
+      <c r="Z263" s="34">
+        <v>0.50782936811447099</v>
+      </c>
       <c r="AA263" s="26">
         <v>7.4000000000000003E-3</v>
       </c>
@@ -26145,6 +26967,9 @@
       <c r="Y264" s="24">
         <v>-5.8</v>
       </c>
+      <c r="Z264" s="34">
+        <v>-0.19357386231422399</v>
+      </c>
       <c r="AA264" s="26">
         <v>3.8E-3</v>
       </c>
@@ -26243,6 +27068,9 @@
       <c r="Y265" s="24">
         <v>-5.6</v>
       </c>
+      <c r="Z265" s="34">
+        <v>0.39221706986427302</v>
+      </c>
       <c r="AA265" s="26">
         <v>2.3999999999999998E-3</v>
       </c>
@@ -26341,6 +27169,9 @@
       <c r="Y266" s="24">
         <v>-6.2</v>
       </c>
+      <c r="Z266" s="34">
+        <v>-0.92031806707382202</v>
+      </c>
       <c r="AA266" s="26">
         <v>6.7999999999999996E-3</v>
       </c>
@@ -26439,6 +27270,9 @@
       <c r="Y267" s="24">
         <v>-6</v>
       </c>
+      <c r="Z267" s="34">
+        <v>-1.3641116619110101</v>
+      </c>
       <c r="AA267" s="26">
         <v>2.5999999999999999E-3</v>
       </c>
@@ -26536,6 +27370,9 @@
       </c>
       <c r="Y268" s="24">
         <v>-5.8</v>
+      </c>
+      <c r="Z268" s="34">
+        <v>-2.2876753807067902</v>
       </c>
       <c r="AA268" s="26">
         <v>6.1999999999999998E-3</v>

</xml_diff>